<commit_message>
add new methods, must fix UT problems
</commit_message>
<xml_diff>
--- a/planning/CalendarEmpty.xlsx
+++ b/planning/CalendarEmpty.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="4" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -21,6 +22,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Content</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -32,12 +41,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -52,8 +67,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -333,7 +351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -341,4 +359,24 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="13" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E13" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>